<commit_message>
add fee and tax
</commit_message>
<xml_diff>
--- a/Data2/Result/daily_performance_0.1_rank_BL.xlsx
+++ b/Data2/Result/daily_performance_0.1_rank_BL.xlsx
@@ -443,7 +443,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2012-01-02</t>
+          <t>2020-01-02</t>
         </is>
       </c>
     </row>
@@ -466,17 +466,17 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>16.2</v>
+        <v>2.65</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.17</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.45</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="9">
@@ -486,17 +486,17 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2.13</v>
+        <v>2.38</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.51</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.3</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="13">
@@ -506,42 +506,42 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>481</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1.31</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.06</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1.3</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.54</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.76</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1.19</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="22">
@@ -551,7 +551,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>4.24</v>
+        <v>4.43</v>
       </c>
     </row>
     <row r="24">
@@ -586,17 +586,17 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.27</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.16</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.17</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="33">
@@ -606,22 +606,22 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>9.43</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>2.43</v>
+        <v>1.53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>